<commit_message>
feat(all): messy commit with work in progress
</commit_message>
<xml_diff>
--- a/fail.xlsx
+++ b/fail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucthomes/Desktop/REPOSITORIES/Glycontact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FEC87B-92CF-F94F-AA35-BCA4494388F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFAE1B4-FE3B-D248-8A08-BABABE73C3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{B99AB1D1-61A9-3340-85EB-C9E4718B2784}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="80">
   <si>
     <t>Gal(b1-4)GlcNAc(b1-2)Man(a1-3)[Gal(b1-4)GlcNAc6S(b1-2)Man(a1-6)]Man(b1-4)GlcNAc(b1-4)[Fuc(a1-6)]GlcNAc</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>Non mais pourquoi ? IdoA2S non reconnu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok </t>
   </si>
 </sst>
 </file>
@@ -638,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B27E90-32F5-D148-BA97-8D83C4DAA9C6}">
   <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,22 +650,28 @@
     <col min="1" max="1" width="73.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -689,93 +698,129 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
         <v>74</v>
@@ -783,7 +828,7 @@
     </row>
     <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
         <v>74</v>
@@ -791,38 +836,47 @@
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
         <v>74</v>
@@ -830,12 +884,15 @@
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
         <v>74</v>
@@ -843,20 +900,23 @@
     </row>
     <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
+      </c>
+      <c r="B33" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
         <v>74</v>
@@ -864,271 +924,223 @@
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+    <row r="68" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
+    <row r="69" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+    <row r="70" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+    <row r="71" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="72" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
+    <row r="73" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B74">
+    <sortCondition ref="B65:B74"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>